<commit_message>
Agregando correccion informe y muestra paralelo en ambos
</commit_message>
<xml_diff>
--- a/Parcial 2/tablas parcial 2.xlsx
+++ b/Parcial 2/tablas parcial 2.xlsx
@@ -553,11 +553,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="311671784"/>
-        <c:axId val="311670216"/>
+        <c:axId val="310482744"/>
+        <c:axId val="310484344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="311671784"/>
+        <c:axId val="310482744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +600,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311670216"/>
+        <c:crossAx val="310484344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -608,7 +608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="311670216"/>
+        <c:axId val="310484344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +715,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311671784"/>
+        <c:crossAx val="310482744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1055,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="328390720"/>
-        <c:axId val="328387976"/>
+        <c:axId val="310484736"/>
+        <c:axId val="310483168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="328390720"/>
+        <c:axId val="310484736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,7 +1102,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328387976"/>
+        <c:crossAx val="310483168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1110,7 +1110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="328387976"/>
+        <c:axId val="310483168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1217,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328390720"/>
+        <c:crossAx val="310484736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1545,11 +1545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="327758584"/>
-        <c:axId val="325787680"/>
+        <c:axId val="310967936"/>
+        <c:axId val="310967152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="327758584"/>
+        <c:axId val="310967936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,7 +1592,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325787680"/>
+        <c:crossAx val="310967152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1600,7 +1600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="325787680"/>
+        <c:axId val="310967152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,7 +1707,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327758584"/>
+        <c:crossAx val="310967936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2116,11 +2116,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="314052576"/>
-        <c:axId val="314051008"/>
+        <c:axId val="310969896"/>
+        <c:axId val="310969112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="314052576"/>
+        <c:axId val="310969896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,7 +2163,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314051008"/>
+        <c:crossAx val="310969112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2171,7 +2171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314051008"/>
+        <c:axId val="310969112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2283,7 +2283,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314052576"/>
+        <c:crossAx val="310969896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4592,16 +4592,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4622,16 +4622,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>795337</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>509587</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>757237</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4652,16 +4652,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>681037</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>776287</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4682,16 +4682,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>671512</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>795337</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4978,8 +4978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5223,7 +5223,7 @@
         <v>26.220860370103331</v>
       </c>
       <c r="S4" s="7">
-        <f t="shared" ref="S4:W4" si="1">C22/C46</f>
+        <f t="shared" ref="S4:U4" si="1">C22/C46</f>
         <v>29.999591419816142</v>
       </c>
       <c r="T4" s="7">
@@ -5295,7 +5295,7 @@
         <v>25.491822429906538</v>
       </c>
       <c r="S5" s="7">
-        <f t="shared" ref="S5:W5" si="2">C22/K46</f>
+        <f t="shared" ref="S5:U5" si="2">C22/K46</f>
         <v>30.843940348666241</v>
       </c>
       <c r="T5" s="7">
@@ -5367,7 +5367,7 @@
         <v>1.4736842105263157</v>
       </c>
       <c r="S6" s="7">
-        <f t="shared" ref="S6:W6" si="3">K22/C46</f>
+        <f t="shared" ref="S6:U6" si="3">K22/C46</f>
         <v>1.4541368743615934</v>
       </c>
       <c r="T6" s="7">
@@ -5439,7 +5439,7 @@
         <v>1.4327102803738319</v>
       </c>
       <c r="S7" s="7">
-        <f t="shared" ref="S7:W7" si="4">K22/K46</f>
+        <f t="shared" ref="S7:U7" si="4">K22/K46</f>
         <v>1.4950640621718123</v>
       </c>
       <c r="T7" s="7">
@@ -5511,7 +5511,7 @@
         <v>0.97219626168224316</v>
       </c>
       <c r="S8" s="7">
-        <f t="shared" ref="S8:W8" si="5">C46/K46</f>
+        <f t="shared" ref="S8:U8" si="5">C46/K46</f>
         <v>1.0281453476160469</v>
       </c>
       <c r="T8" s="7">

</xml_diff>

<commit_message>
Agregando grafico de barras
</commit_message>
<xml_diff>
--- a/Parcial 2/tablas parcial 2.xlsx
+++ b/Parcial 2/tablas parcial 2.xlsx
@@ -553,11 +553,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="310482744"/>
-        <c:axId val="310484344"/>
+        <c:axId val="140247584"/>
+        <c:axId val="140248368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="310482744"/>
+        <c:axId val="140247584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +600,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310484344"/>
+        <c:crossAx val="140248368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -608,7 +608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310484344"/>
+        <c:axId val="140248368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +715,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310482744"/>
+        <c:crossAx val="140247584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1055,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="310484736"/>
-        <c:axId val="310483168"/>
+        <c:axId val="140249152"/>
+        <c:axId val="140249544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="310484736"/>
+        <c:axId val="140249152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,7 +1102,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310483168"/>
+        <c:crossAx val="140249544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1110,7 +1110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310483168"/>
+        <c:axId val="140249544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1217,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310484736"/>
+        <c:crossAx val="140249152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1545,11 +1545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="310967936"/>
-        <c:axId val="310967152"/>
+        <c:axId val="140247976"/>
+        <c:axId val="110189968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="310967936"/>
+        <c:axId val="140247976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,7 +1592,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310967152"/>
+        <c:crossAx val="110189968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1600,7 +1600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310967152"/>
+        <c:axId val="110189968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,7 +1707,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310967936"/>
+        <c:crossAx val="140247976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2116,11 +2116,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="310969896"/>
-        <c:axId val="310969112"/>
+        <c:axId val="110189576"/>
+        <c:axId val="110190360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="310969896"/>
+        <c:axId val="110189576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,7 +2163,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310969112"/>
+        <c:crossAx val="110190360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2171,7 +2171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="310969112"/>
+        <c:axId val="110190360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2283,7 +2283,613 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="310969896"/>
+        <c:crossAx val="110189576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Aceleraciones</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>secuencial global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$2:$W$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>img1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>img2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>img3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>img4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>img6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>img5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$3:$W$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>17.792726679712978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.630514189379038</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.188404911723381</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.409504637037806</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.567055493414301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.195225944522186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>secuencial constante</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$2:$W$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>img1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>img2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>img3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>img4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>img6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>img5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$4:$W$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>26.220860370103331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.999591419816142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.928225576758763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.498654859320709</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.201028057077494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.164984260173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>secuencial compartida</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$2:$W$2</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>img1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>img2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>img3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>img4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>img6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>img5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$5:$W$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>25.491822429906538</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.843940348666241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.432485505891151</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.884200390813064</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.720166107033556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.448422031543153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="332848064"/>
+        <c:axId val="332849240"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="332848064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="332849240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="332849240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Cantidad de veces</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CO" baseline="0"/>
+                  <a:t> aceleradas(X's)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="332848064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2524,6 +3130,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4556,6 +5202,500 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4710,6 +5850,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4979,7 +6149,7 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="Q2" sqref="Q2:W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>